<commit_message>
Creación del modulo para incrementos de salarios
</commit_message>
<xml_diff>
--- a/data/plantilla_laboral2.xlsx
+++ b/data/plantilla_laboral2.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cursos\z_proyectos\nomina_2\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="6735"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -294,6 +299,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -341,7 +349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,7 +384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +596,7 @@
   <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
creación de un notebook para calculos imss -todo ok
</commit_message>
<xml_diff>
--- a/data/plantilla_laboral2.xlsx
+++ b/data/plantilla_laboral2.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="6735" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$55</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -502,7 +505,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -510,7 +513,6 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -823,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B55"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -833,7 +835,7 @@
     <col min="4" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -850,7 +852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -866,8 +868,10 @@
       <c r="E2" s="6">
         <v>43619</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -883,8 +887,10 @@
       <c r="E3" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>6</v>
       </c>
@@ -900,8 +906,10 @@
       <c r="E4" s="6">
         <v>43669</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>7</v>
       </c>
@@ -917,8 +925,10 @@
       <c r="E5" s="6">
         <v>43528</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>8</v>
       </c>
@@ -934,8 +944,10 @@
       <c r="E6" s="6">
         <v>43109</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>9</v>
       </c>
@@ -951,8 +963,10 @@
       <c r="E7" s="6">
         <v>42194</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>11</v>
       </c>
@@ -968,8 +982,10 @@
       <c r="E8" s="6">
         <v>43132</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>12</v>
       </c>
@@ -985,8 +1001,10 @@
       <c r="E9" s="6">
         <v>43409</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>13</v>
       </c>
@@ -1002,8 +1020,10 @@
       <c r="E10" s="6">
         <v>43710</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>14</v>
       </c>
@@ -1019,8 +1039,10 @@
       <c r="E11" s="6">
         <v>43124</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>15</v>
       </c>
@@ -1036,8 +1058,10 @@
       <c r="E12" s="6">
         <v>43360</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>18</v>
       </c>
@@ -1053,8 +1077,10 @@
       <c r="E13" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>19</v>
       </c>
@@ -1070,8 +1096,10 @@
       <c r="E14" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>21</v>
       </c>
@@ -1087,8 +1115,10 @@
       <c r="E15" s="6">
         <v>42186</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>23</v>
       </c>
@@ -1104,8 +1134,10 @@
       <c r="E16" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>24</v>
       </c>
@@ -1121,8 +1153,10 @@
       <c r="E17" s="6">
         <v>43770</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>25</v>
       </c>
@@ -1138,8 +1172,10 @@
       <c r="E18" s="6">
         <v>43619</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>26</v>
       </c>
@@ -1155,8 +1191,10 @@
       <c r="E19" s="6">
         <v>42385</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>27</v>
       </c>
@@ -1172,8 +1210,10 @@
       <c r="E20" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>28</v>
       </c>
@@ -1189,8 +1229,10 @@
       <c r="E21" s="6">
         <v>42156</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>29</v>
       </c>
@@ -1206,8 +1248,10 @@
       <c r="E22" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>30</v>
       </c>
@@ -1223,8 +1267,10 @@
       <c r="E23" s="6">
         <v>41579</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>31</v>
       </c>
@@ -1240,8 +1286,10 @@
       <c r="E24" s="6">
         <v>43409</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>33</v>
       </c>
@@ -1257,8 +1305,10 @@
       <c r="E25" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>35</v>
       </c>
@@ -1274,8 +1324,10 @@
       <c r="E26" s="6">
         <v>42548</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>36</v>
       </c>
@@ -1291,8 +1343,10 @@
       <c r="E27" s="6">
         <v>41659</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
         <v>38</v>
       </c>
@@ -1308,8 +1362,10 @@
       <c r="E28" s="6">
         <v>44025</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
         <v>40</v>
       </c>
@@ -1325,8 +1381,10 @@
       <c r="E29" s="6">
         <v>44112</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
         <v>41</v>
       </c>
@@ -1342,8 +1400,10 @@
       <c r="E30" s="6">
         <v>43116</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
         <v>42</v>
       </c>
@@ -1354,13 +1414,15 @@
         <v>29228.38</v>
       </c>
       <c r="D31" s="5">
-        <v>1169</v>
+        <v>1461</v>
       </c>
       <c r="E31" s="6">
         <v>43632</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>43</v>
       </c>
@@ -1376,8 +1438,10 @@
       <c r="E32" s="6">
         <v>43472</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>44</v>
       </c>
@@ -1393,8 +1457,10 @@
       <c r="E33" s="6">
         <v>43633</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="2">
         <v>46</v>
       </c>
@@ -1410,8 +1476,10 @@
       <c r="E34" s="6">
         <v>44378</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>48</v>
       </c>
@@ -1427,8 +1495,10 @@
       <c r="E35" s="6">
         <v>43080</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
         <v>49</v>
       </c>
@@ -1444,8 +1514,10 @@
       <c r="E36" s="6">
         <v>43497</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
         <v>50</v>
       </c>
@@ -1461,8 +1533,10 @@
       <c r="E37" s="6">
         <v>43612</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
         <v>51</v>
       </c>
@@ -1478,8 +1552,10 @@
       <c r="E38" s="6">
         <v>44044</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="2">
         <v>52</v>
       </c>
@@ -1495,8 +1571,10 @@
       <c r="E39" s="6">
         <v>44075</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="2">
         <v>53</v>
       </c>
@@ -1512,8 +1590,10 @@
       <c r="E40" s="6">
         <v>44440</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="2">
         <v>55</v>
       </c>
@@ -1529,8 +1609,10 @@
       <c r="E41" s="6">
         <v>44577</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
         <v>56</v>
       </c>
@@ -1546,8 +1628,10 @@
       <c r="E42" s="6">
         <v>44593</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="2">
         <v>57</v>
       </c>
@@ -1563,8 +1647,10 @@
       <c r="E43" s="6">
         <v>44593</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>58</v>
       </c>
@@ -1580,8 +1666,10 @@
       <c r="E44" s="6">
         <v>44610</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="2">
         <v>59</v>
       </c>
@@ -1597,8 +1685,10 @@
       <c r="E45" s="6">
         <v>44621</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>60</v>
       </c>
@@ -1614,8 +1704,10 @@
       <c r="E46" s="6">
         <v>44697</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="2">
         <v>61</v>
       </c>
@@ -1631,8 +1723,10 @@
       <c r="E47" s="6">
         <v>44697</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="2">
         <v>62</v>
       </c>
@@ -1648,6 +1742,8 @@
       <c r="E48" s="6">
         <v>44713</v>
       </c>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2">
@@ -1665,6 +1761,8 @@
       <c r="E49" s="6">
         <v>44728</v>
       </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2">
@@ -1682,6 +1780,8 @@
       <c r="E50" s="6">
         <v>44728</v>
       </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2">
@@ -1699,6 +1799,8 @@
       <c r="E51" s="6">
         <v>44728</v>
       </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2">
@@ -1716,6 +1818,8 @@
       <c r="E52" s="6">
         <v>44743</v>
       </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2">
@@ -1733,7 +1837,8 @@
       <c r="E53" s="6">
         <v>44795</v>
       </c>
-      <c r="G53" s="7"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2">
@@ -1751,8 +1856,8 @@
       <c r="E54" s="6">
         <v>44823</v>
       </c>
-      <c r="G54" s="7"/>
-      <c r="H54" s="1"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2">
@@ -1770,11 +1875,12 @@
       <c r="E55" s="6">
         <v>44896</v>
       </c>
-      <c r="G55" s="7"/>
-      <c r="H55" s="1"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1788,37 +1894,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="9"/>
+    <col min="1" max="1" width="17.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>27000</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <f>INT(B3*0.0476)</f>
         <v>1285</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f>B3-B4</f>
         <v>25715</v>
       </c>
@@ -1833,670 +1939,670 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E71" sqref="E3:E71"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="8" width="11.42578125" style="11"/>
-    <col min="9" max="9" width="29.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="8" width="11.42578125" style="10"/>
+    <col min="9" max="9" width="29.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:5">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E3" s="11" t="str">
+      <c r="E3" s="10" t="str">
         <f t="shared" ref="E3:E58" si="0">"MD "&amp;C3</f>
         <v>MD Adela_Marin_Castillo_-3437</v>
       </c>
     </row>
     <row r="4" spans="3:5">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="11" t="str">
+      <c r="E4" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ana_Gomez_Gallardo_Aguilar_-0538-4646</v>
       </c>
     </row>
     <row r="5" spans="3:5">
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="11" t="str">
+      <c r="E5" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ana_Norely_Flores_Robles_-2744</v>
       </c>
     </row>
     <row r="6" spans="3:5">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="11" t="str">
+      <c r="E6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ana_Paula_Gout_Martinez_de_Velasco_-2769</v>
       </c>
     </row>
     <row r="7" spans="3:5">
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="11" t="str">
+      <c r="E7" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Andres_Pena_Peralta_-4620-5436</v>
       </c>
     </row>
     <row r="8" spans="3:5">
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Angel_Manuel_Ramirez_Contreras_-3429</v>
       </c>
     </row>
     <row r="9" spans="3:5">
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="E9" s="11" t="str">
+      <c r="E9" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Blanca_Elena_Leiva_Lopez_-4881</v>
       </c>
     </row>
     <row r="10" spans="3:5">
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="11" t="str">
+      <c r="E10" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Brenda_Bernaldez_Ruiz_-2629</v>
       </c>
     </row>
     <row r="11" spans="3:5">
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="11" t="str">
+      <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Brenda_Hernandez_Jimenez_-3332</v>
       </c>
     </row>
     <row r="12" spans="3:5">
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="11" t="str">
+      <c r="E12" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Dulce_Nelida_Martinez_Ruvalcaba_-0983</v>
       </c>
     </row>
     <row r="13" spans="3:5">
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="11" t="str">
+      <c r="E13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Elias_Ebeth_Teco_Sanchez_-7818</v>
       </c>
     </row>
     <row r="14" spans="3:5">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="11" t="str">
+      <c r="E14" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Elias_Trinidad_Ramos_Razo_-3627</v>
       </c>
     </row>
     <row r="15" spans="3:5">
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E15" s="11" t="str">
+      <c r="E15" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Estela_Herrera_Gonzalez_-0187-3537</v>
       </c>
     </row>
     <row r="16" spans="3:5">
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="11" t="str">
+      <c r="E16" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ethel_Edith_Montoya_Crespo_-3593</v>
       </c>
     </row>
     <row r="17" spans="3:5">
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="11" t="str">
+      <c r="E17" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Francisco_Perez_Gaspar_-3643</v>
       </c>
     </row>
     <row r="18" spans="3:5">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="11" t="str">
+      <c r="E18" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Gerardo_Gonzalez_Flores</v>
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="11" t="str">
+      <c r="E19" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ismael_Martinez_Gallegos_-1757</v>
       </c>
     </row>
     <row r="20" spans="3:5">
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="11" t="str">
+      <c r="E20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Jesus_Ruvalcaba_Mota_-5077</v>
       </c>
     </row>
     <row r="21" spans="3:5">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="11" t="str">
+      <c r="E21" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Jonathan_Covarrubias_Sustaita_-2694</v>
       </c>
     </row>
     <row r="22" spans="3:5">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="11" t="str">
+      <c r="E22" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Jose_Alfredo_Lopez_Madrigal_-3695</v>
       </c>
     </row>
     <row r="23" spans="3:5">
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="11" t="str">
+      <c r="E23" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Jose_Manuel_Franco_Gonzalez_-2678</v>
       </c>
     </row>
     <row r="24" spans="3:5">
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="11" t="str">
+      <c r="E24" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Jose_Maria_Sandoval_Torres_-3668</v>
       </c>
     </row>
     <row r="25" spans="3:5">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E25" s="11" t="str">
+      <c r="E25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Josue_Leon_Morales_-2652</v>
       </c>
     </row>
     <row r="26" spans="3:5">
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="11" t="str">
+      <c r="E26" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Juan_Gonzalez_Barajas_-0513</v>
       </c>
     </row>
     <row r="27" spans="3:5">
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="11" t="str">
+      <c r="E27" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Juan_Gonzalez_Barajas_-0553</v>
       </c>
     </row>
     <row r="28" spans="3:5">
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="11" t="str">
+      <c r="E28" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Juan_Gonzalez_Barajas_-0626</v>
       </c>
     </row>
     <row r="29" spans="3:5">
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="11" t="str">
+      <c r="E29" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Juan_Gonzalez_Barajas_-7220</v>
       </c>
     </row>
     <row r="30" spans="3:5">
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="11" t="str">
+      <c r="E30" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Karen_Alejandra_Lara_Paz</v>
       </c>
     </row>
     <row r="31" spans="3:5">
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="11" t="str">
+      <c r="E31" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Karla_Cano_Garcia_-4437-9079</v>
       </c>
     </row>
     <row r="32" spans="3:5">
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E32" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Katya_del_Rocio_Lopez_Ramirez_-7573</v>
       </c>
     </row>
     <row r="33" spans="3:5">
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="11" t="str">
+      <c r="E33" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Luis_Manuel_Guerrero_Alcantara</v>
       </c>
     </row>
     <row r="34" spans="3:5">
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E34" s="11" t="str">
+      <c r="E34" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Manuel_Alejandro_Monroy_Cruz_-3460</v>
       </c>
     </row>
     <row r="35" spans="3:5">
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="11" t="str">
+      <c r="E35" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Margaux_Andree_B_Jacquemin_X_-7651</v>
       </c>
     </row>
     <row r="36" spans="3:5">
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E36" s="11" t="str">
+      <c r="E36" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Maria_Alejandra_Torres_Sandoval_-7826</v>
       </c>
     </row>
     <row r="37" spans="3:5">
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="11" t="str">
+      <c r="E37" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Maria_del_Pilar_Velez_Jimenez_-3635</v>
       </c>
     </row>
     <row r="38" spans="3:5">
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="11" t="str">
+      <c r="E38" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Maria_del_Carmen_Tamayo_Sanchez_Mejorada_</v>
       </c>
     </row>
     <row r="39" spans="3:5">
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="11" t="str">
+      <c r="E39" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Mariana_Ramirez_Castillo_-4873</v>
       </c>
     </row>
     <row r="40" spans="3:5">
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="11" t="str">
+      <c r="E40" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Martha_Rosa_Alvarez_Martinez_-4824</v>
       </c>
     </row>
     <row r="41" spans="3:5">
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="11" t="str">
+      <c r="E41" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Miguel_Dionicio_Luna_-5196</v>
       </c>
     </row>
     <row r="42" spans="3:5">
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E42" s="11" t="str">
+      <c r="E42" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Monica_Alvarado_Espindola</v>
       </c>
     </row>
     <row r="43" spans="3:5">
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E43" s="11" t="str">
+      <c r="E43" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Monica_Gonzalez_Garduno_-0512</v>
       </c>
     </row>
     <row r="44" spans="3:5">
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="11" t="str">
+      <c r="E44" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Nayeli_Melisa_Rodriguez_Leonardo_-7789</v>
       </c>
     </row>
     <row r="45" spans="3:5">
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="11" t="str">
+      <c r="E45" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ricardo_Chavez_Rebollo_-3111</v>
       </c>
     </row>
     <row r="46" spans="3:5">
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E46" s="11" t="str">
+      <c r="E46" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Ricardo_Neri_Vazquez_-4633</v>
       </c>
     </row>
     <row r="47" spans="3:5">
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="11" t="str">
+      <c r="E47" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Rogelio_Cervantes_Moreno_-2728</v>
       </c>
     </row>
     <row r="48" spans="3:5">
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="11" t="str">
+      <c r="E48" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Rosa_Isela_Gallegos_Orozco</v>
       </c>
     </row>
     <row r="49" spans="2:5">
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E49" s="11" t="str">
+      <c r="E49" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Rosa_Juarez_Pinzon_-376</v>
       </c>
     </row>
     <row r="50" spans="2:5">
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E50" s="11" t="str">
+      <c r="E50" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Samantha_Martinez_Narcizo_-3445</v>
       </c>
     </row>
     <row r="51" spans="2:5">
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="11" t="str">
+      <c r="E51" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Sarai_Rosas_Trujillo_-2637</v>
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="11" t="str">
+      <c r="E52" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Sergio_Moreno_Gonzalez_-2736</v>
       </c>
     </row>
     <row r="53" spans="2:5">
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E53" s="11" t="str">
+      <c r="E53" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Sergio_Alexis_Bautista_Angeles</v>
       </c>
     </row>
     <row r="54" spans="2:5">
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E54" s="11" t="str">
+      <c r="E54" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Shaila_Barradas_Santiago</v>
       </c>
     </row>
     <row r="55" spans="2:5">
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="E55" s="11" t="str">
+      <c r="E55" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Stephany_Peniche_Ake_-3403</v>
       </c>
     </row>
     <row r="56" spans="2:5">
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E56" s="11" t="str">
+      <c r="E56" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Susana_Garza_Leon_-3486</v>
       </c>
     </row>
     <row r="57" spans="2:5">
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="11" t="str">
+      <c r="E57" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Tania_Monserrat_Banuelos_Murillo_-4840</v>
       </c>
     </row>
     <row r="58" spans="2:5">
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="E58" s="11" t="str">
+      <c r="E58" s="10" t="str">
         <f t="shared" si="0"/>
         <v>MD Tania_Alejandra_Lopez_Conde_Cervantes_-3452</v>
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E59" s="11" t="str">
+      <c r="E59" s="10" t="str">
         <f>"MD "&amp;C59</f>
         <v>MD Zurisadai_Arano_Rivera_-3411</v>
       </c>
     </row>
     <row r="60" spans="2:5">
-      <c r="B60" s="11">
+      <c r="B60" s="10">
         <v>1</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="11" t="str">
-        <f>"MD 0"&amp;B60&amp;"_"&amp;C60</f>
+      <c r="E60" s="10" t="str">
+        <f t="shared" ref="E60:E68" si="1">"MD 0"&amp;B60&amp;"_"&amp;C60</f>
         <v>MD 01_Enero</v>
       </c>
     </row>
     <row r="61" spans="2:5">
-      <c r="B61" s="11">
+      <c r="B61" s="10">
         <v>2</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="11" t="str">
-        <f>"MD 0"&amp;B61&amp;"_"&amp;C61</f>
+      <c r="E61" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 02_Febrero</v>
       </c>
     </row>
     <row r="62" spans="2:5">
-      <c r="B62" s="11">
+      <c r="B62" s="10">
         <v>3</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E62" s="11" t="str">
-        <f>"MD 0"&amp;B62&amp;"_"&amp;C62</f>
+      <c r="E62" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 03_Marzo</v>
       </c>
     </row>
     <row r="63" spans="2:5">
-      <c r="B63" s="11">
+      <c r="B63" s="10">
         <v>4</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E63" s="11" t="str">
-        <f>"MD 0"&amp;B63&amp;"_"&amp;C63</f>
+      <c r="E63" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 04_Abril</v>
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="11">
+      <c r="B64" s="10">
         <v>5</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E64" s="11" t="str">
-        <f>"MD 0"&amp;B64&amp;"_"&amp;C64</f>
+      <c r="E64" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 05_Mayo</v>
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="11">
+      <c r="B65" s="10">
         <v>6</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E65" s="11" t="str">
-        <f>"MD 0"&amp;B65&amp;"_"&amp;C65</f>
+      <c r="E65" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 06_Junio</v>
       </c>
     </row>
     <row r="66" spans="2:5">
-      <c r="B66" s="11">
+      <c r="B66" s="10">
         <v>7</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E66" s="11" t="str">
-        <f>"MD 0"&amp;B66&amp;"_"&amp;C66</f>
+      <c r="E66" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 07_Julio</v>
       </c>
     </row>
     <row r="67" spans="2:5">
-      <c r="B67" s="11">
+      <c r="B67" s="10">
         <v>8</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E67" s="11" t="str">
-        <f>"MD 0"&amp;B67&amp;"_"&amp;C67</f>
+      <c r="E67" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 08_Agosto</v>
       </c>
     </row>
     <row r="68" spans="2:5">
-      <c r="B68" s="11">
+      <c r="B68" s="10">
         <v>9</v>
       </c>
-      <c r="C68" s="11" t="s">
+      <c r="C68" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E68" s="11" t="str">
-        <f>"MD 0"&amp;B68&amp;"_"&amp;C68</f>
+      <c r="E68" s="10" t="str">
+        <f t="shared" si="1"/>
         <v>MD 09_Septiembre</v>
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="11">
+      <c r="B69" s="10">
         <v>10</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E69" s="11" t="str">
+      <c r="E69" s="10" t="str">
         <f>"MD "&amp;B69&amp;"_"&amp;C69</f>
         <v>MD 10_Octubre</v>
       </c>
     </row>
     <row r="70" spans="2:5">
-      <c r="B70" s="11">
+      <c r="B70" s="10">
         <v>11</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="C70" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E70" s="11" t="str">
+      <c r="E70" s="10" t="str">
         <f>"MD "&amp;B70&amp;"_"&amp;C70</f>
         <v>MD 11_Noviembre</v>
       </c>
     </row>
     <row r="71" spans="2:5">
-      <c r="B71" s="11">
+      <c r="B71" s="10">
         <v>12</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E71" s="11" t="str">
+      <c r="E71" s="10" t="str">
         <f>"MD "&amp;B71&amp;"_"&amp;C71</f>
         <v>MD 12_Diciembre</v>
       </c>

</xml_diff>

<commit_message>
calculos de columnas del dataframe del 2022 al 2023 del modulo clean_load
</commit_message>
<xml_diff>
--- a/data/plantilla_laboral2.xlsx
+++ b/data/plantilla_laboral2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="6735" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="10515" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -902,7 +902,7 @@
     <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,6 +984,11 @@
       <color rgb="FF000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u val="singleAccounting"/>
+      <sz val="8"/>
+      <name val="Verdena"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1144,7 +1149,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1220,6 +1225,7 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1539,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2516,7 +2522,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" ht="16.5">
       <c r="A52" s="2">
         <v>66</v>
       </c>
@@ -2532,7 +2538,7 @@
       <c r="E52" s="6">
         <v>44743</v>
       </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="35"/>
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8">
@@ -2543,10 +2549,10 @@
         <v>54</v>
       </c>
       <c r="C53" s="5">
-        <v>19500.080000000002</v>
+        <v>21717.75</v>
       </c>
       <c r="D53" s="5">
-        <v>975</v>
+        <v>1086</v>
       </c>
       <c r="E53" s="6">
         <v>44795</v>
@@ -2602,7 +2608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -4159,11 +4165,11 @@
       </c>
       <c r="M23" s="33">
         <f>VLOOKUP(C23,Hoja1!$A$2:$C$55,3,0)</f>
-        <v>19500.080000000002</v>
+        <v>21717.75</v>
       </c>
       <c r="N23" s="34">
         <f t="shared" ref="N23:N25" si="2">K23-M23</f>
-        <v>0</v>
+        <v>-2217.6699999999983</v>
       </c>
     </row>
     <row r="24" spans="3:14">

</xml_diff>

<commit_message>
to pull origin master
</commit_message>
<xml_diff>
--- a/data/plantilla_laboral2.xlsx
+++ b/data/plantilla_laboral2.xlsx
@@ -896,11 +896,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1149,7 +1150,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1226,6 +1227,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1543,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2465,7 +2467,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>63</v>
       </c>
@@ -2484,7 +2486,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>64</v>
       </c>
@@ -2503,7 +2505,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:9">
       <c r="A51" s="2">
         <v>65</v>
       </c>
@@ -2522,7 +2524,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="16.5">
+    <row r="52" spans="1:9" ht="16.5">
       <c r="A52" s="2">
         <v>66</v>
       </c>
@@ -2541,7 +2543,7 @@
       <c r="G52" s="35"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9">
       <c r="A53" s="2">
         <v>67</v>
       </c>
@@ -2560,7 +2562,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>68</v>
       </c>
@@ -2579,7 +2581,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:9">
       <c r="A55" s="2">
         <v>69</v>
       </c>
@@ -2597,6 +2599,10 @@
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
+      <c r="I55" s="36"/>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="I56" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ultimos cambios fondo de ahorro
</commit_message>
<xml_diff>
--- a/data/plantilla_laboral2.xlsx
+++ b/data/plantilla_laboral2.xlsx
@@ -901,7 +901,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -1227,7 +1227,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1547,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2399,7 +2399,8 @@
         <v>46</v>
       </c>
       <c r="C45" s="5">
-        <v>5255.24</v>
+        <f>207.44*30.4</f>
+        <v>6306.1759999999995</v>
       </c>
       <c r="D45" s="5">
         <v>263</v>
@@ -3912,11 +3913,11 @@
       </c>
       <c r="M16" s="33">
         <f>VLOOKUP(C16,Hoja1!$A$2:$C$55,3,0)</f>
-        <v>5255.24</v>
+        <v>6306.1759999999995</v>
       </c>
       <c r="N16" s="34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1050.9359999999997</v>
       </c>
     </row>
     <row r="17" spans="3:14">

</xml_diff>